<commit_message>
Start Forms by Prathamesh
</commit_message>
<xml_diff>
--- a/clientdata/Forms And Its Fields.xlsx
+++ b/clientdata/Forms And Its Fields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -573,9 +573,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -596,9 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -652,6 +646,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,12 +968,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -990,114 +990,114 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="24" t="b">
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24" t="b">
+      <c r="D5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24" t="b">
+      <c r="D6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="23" t="b">
+      <c r="D7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="24" t="b">
+      <c r="D8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>6</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24" t="b">
+      <c r="D9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>7</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="24" t="b">
+      <c r="D10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>8</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="24" t="b">
+      <c r="D11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1114,31 +1114,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="60.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1149,116 +1149,116 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
-        <v>1</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="24" t="b">
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24" t="b">
+      <c r="D5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24" t="b">
+      <c r="D6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="24" t="b">
+      <c r="D7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="24" t="b">
+      <c r="D8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>6</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24" t="b">
+      <c r="D9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>7</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="23" t="b">
+      <c r="D10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1269,144 +1269,144 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="20">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="24" t="b">
+      <c r="D14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="22">
+      <c r="B15" s="20">
         <v>2</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="24" t="b">
+      <c r="D15" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="22">
+      <c r="B16" s="20">
         <v>3</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="24" t="b">
+      <c r="D16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
+      <c r="B17" s="20">
         <v>4</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24" t="b">
+      <c r="D17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>5</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="24" t="b">
+      <c r="D18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>6</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="24" t="b">
+      <c r="D19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>7</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24" t="b">
+      <c r="D20" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+      <c r="B21" s="20">
         <v>8</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24" t="b">
+      <c r="D21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
+      <c r="B22" s="20">
         <v>9</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24" t="b">
+      <c r="D22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1417,200 +1417,200 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="22">
-        <v>1</v>
-      </c>
-      <c r="C26" s="25" t="s">
+      <c r="B26" s="20">
+        <v>1</v>
+      </c>
+      <c r="C26" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24" t="b">
+      <c r="D26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="22">
+      <c r="B27" s="20">
         <v>2</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="24" t="b">
+      <c r="D27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="22">
+      <c r="B28" s="20">
         <v>3</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="24" t="b">
+      <c r="D28" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="22">
+      <c r="B29" s="20">
         <v>4</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="24" t="b">
+      <c r="D29" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="22">
+      <c r="B30" s="20">
         <v>5</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="24" t="b">
+      <c r="D30" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="22">
+      <c r="B31" s="20">
         <v>6</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="24" t="b">
+      <c r="D31" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="22">
+      <c r="B32" s="20">
         <v>7</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="24" t="b">
+      <c r="D32" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="22">
+      <c r="B33" s="20">
         <v>8</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24" t="b">
+      <c r="D33" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="22">
+      <c r="B34" s="20">
         <v>9</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="24" t="b">
+      <c r="D34" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="22">
+      <c r="B35" s="20">
         <v>10</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24" t="b">
+      <c r="D35" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="22">
+      <c r="B36" s="20">
         <v>11</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="24" t="b">
+      <c r="D36" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="22">
+      <c r="B37" s="20">
         <v>12</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="24" t="b">
+      <c r="D37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="22">
+      <c r="B38" s="20">
         <v>13</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="24" t="b">
+      <c r="D38" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1621,44 +1621,44 @@
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="22">
-        <v>1</v>
-      </c>
-      <c r="C42" s="25" t="s">
+      <c r="B42" s="20">
+        <v>1</v>
+      </c>
+      <c r="C42" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="24" t="b">
+      <c r="D42" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="22">
+      <c r="B43" s="20">
         <v>2</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="24" t="b">
+      <c r="D43" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="22">
+      <c r="B44" s="20">
         <v>3</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="24" t="b">
+      <c r="D44" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1677,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,18 +1689,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1711,158 +1711,158 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="24" t="b">
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24" t="b">
+      <c r="D5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24" t="b">
+      <c r="D6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="24" t="b">
+      <c r="D7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="23" t="b">
+      <c r="D8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>6</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24" t="b">
+      <c r="D9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>7</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="24" t="b">
+      <c r="D10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>8</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="24" t="b">
+      <c r="D11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>9</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="24" t="b">
+      <c r="D12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>10</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="24" t="b">
+      <c r="D13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1873,128 +1873,128 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24" t="b">
+      <c r="D17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="24" t="b">
+      <c r="D18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="24" t="b">
+      <c r="D19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>4</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24" t="b">
+      <c r="D20" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+      <c r="B21" s="20">
         <v>5</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24" t="b">
+      <c r="D21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
+      <c r="B22" s="20">
         <v>6</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24" t="b">
+      <c r="D22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="22">
+      <c r="B23" s="20">
         <v>7</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="24" t="b">
+      <c r="D23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="22">
+      <c r="B24" s="20">
         <v>8</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="24" t="b">
+      <c r="D24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="22">
+      <c r="B25" s="20">
         <v>9</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="24" t="b">
+      <c r="D25" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2011,30 +2011,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="76.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2045,158 +2045,158 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="20">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="24" t="b">
+      <c r="D4" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24" t="b">
+      <c r="D5" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24" t="b">
+      <c r="D6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="24" t="b">
+      <c r="D7" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="24" t="b">
+      <c r="D8" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24" t="b">
+      <c r="D9" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="24" t="b">
+      <c r="D10" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="24" t="b">
+      <c r="D11" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="24" t="b">
+      <c r="D12" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
+      <c r="B13" s="20">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="24" t="b">
+      <c r="D13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2207,200 +2207,200 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="22">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24" t="b">
+      <c r="D17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="22">
+      <c r="B18" s="20">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="24" t="b">
+      <c r="D18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>3</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="24" t="b">
+      <c r="D19" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="22">
+      <c r="B20" s="20">
         <v>4</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24" t="b">
+      <c r="D20" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
+      <c r="B21" s="20">
         <v>5</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="24" t="b">
+      <c r="D21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="22">
+      <c r="B22" s="20">
         <v>6</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="24" t="b">
+      <c r="D22" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="22">
+      <c r="B23" s="20">
         <v>7</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="24" t="b">
+      <c r="D23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="22">
+      <c r="B24" s="20">
         <v>8</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="24" t="b">
+      <c r="D24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="22">
+      <c r="B25" s="20">
         <v>9</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="24" t="b">
+      <c r="D25" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="22">
+      <c r="B26" s="20">
         <v>10</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24" t="b">
+      <c r="D26" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="22">
+      <c r="B27" s="20">
         <v>11</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="24" t="b">
+      <c r="D27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="22">
+      <c r="B28" s="20">
         <v>12</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="24" t="b">
+      <c r="D28" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="22">
+      <c r="B29" s="20">
         <v>13</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="24" t="b">
+      <c r="D29" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2411,240 +2411,240 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="22">
-        <v>1</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="20">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24" t="b">
+      <c r="D33" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="22">
+      <c r="B34" s="20">
         <v>2</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="24" t="b">
+      <c r="D34" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="22">
+      <c r="B35" s="20">
         <v>3</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="24" t="b">
+      <c r="D35" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="22">
+      <c r="B36" s="20">
         <v>4</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="24" t="b">
+      <c r="D36" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="22">
+      <c r="B37" s="20">
         <v>5</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="24" t="b">
+      <c r="D37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="22">
+      <c r="B38" s="20">
         <v>6</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D38" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="24" t="b">
+      <c r="D38" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="22">
+      <c r="B39" s="20">
         <v>7</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="24" t="b">
+      <c r="D39" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="22">
+      <c r="B40" s="20">
         <v>8</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="23" t="b">
+      <c r="D40" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="22">
+      <c r="B41" s="20">
         <v>9</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="24" t="b">
+      <c r="D41" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="22">
+      <c r="B42" s="20">
         <v>10</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="24" t="b">
+      <c r="D42" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="22">
+      <c r="B43" s="20">
         <v>11</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="24" t="b">
+      <c r="D43" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="22">
+      <c r="B44" s="20">
         <v>12</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="24" t="b">
+      <c r="D44" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="22">
+      <c r="B45" s="20">
         <v>13</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="24" t="b">
+      <c r="D45" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="22">
+      <c r="B46" s="20">
         <v>14</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D46" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="24" t="b">
+      <c r="D46" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="22">
+      <c r="B47" s="20">
         <v>15</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" s="24" t="b">
+      <c r="D47" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="22">
+      <c r="B48" s="20">
         <v>16</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D48" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="24" t="b">
+      <c r="D48" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" s="22" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="22">
+      <c r="B49" s="20">
         <v>17</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="23" t="b">
+      <c r="D49" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="21" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2662,254 +2662,254 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="58.28515625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="15" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="28" t="b">
+      <c r="D4" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="28" t="b">
+      <c r="D5" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="26">
+      <c r="B6" s="24">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28" t="b">
+      <c r="D6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="28" t="b">
+      <c r="D7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="26">
+      <c r="B8" s="24">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="28" t="b">
+      <c r="D8" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="28" t="b">
+      <c r="D9" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="26">
+      <c r="B10" s="24">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="28" t="b">
+      <c r="D10" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="28" t="b">
+      <c r="D11" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="26">
+      <c r="B12" s="24">
         <v>9</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28" t="b">
+      <c r="D12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16" t="b">
+      <c r="D16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="16" t="b">
+      <c r="D17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="16" t="b">
+      <c r="D18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="16" t="b">
+      <c r="D19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>5</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="16" t="b">
+      <c r="D20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2927,119 +2927,119 @@
   <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E9"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="58.42578125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" style="29" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="32">
+      <c r="B4" s="30">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16" t="b">
+      <c r="D4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="16" t="b">
+      <c r="D5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
+      <c r="B6" s="30">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16" t="b">
+      <c r="D6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="32">
+      <c r="B7" s="30">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16" t="b">
+      <c r="D7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="32">
+      <c r="B8" s="30">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16" t="b">
+      <c r="D8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="31">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="15" t="b">
+      <c r="D9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3056,116 +3056,116 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="58.5703125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="58.5703125" style="29" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
+      <c r="B4" s="20">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="28" t="b">
+      <c r="D4" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="28" t="b">
+      <c r="D5" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28" t="b">
+      <c r="D6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="28" t="b">
+      <c r="D7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="28" t="b">
+      <c r="D8" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="26" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>

</xml_diff>